<commit_message>
Python Introduction and Intermediate Uploded
</commit_message>
<xml_diff>
--- a/Data Scientist with Python.xlsx
+++ b/Data Scientist with Python.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$D$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$E$30</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="36">
   <si>
     <t>Data Scientist with Python</t>
   </si>
@@ -133,6 +133,9 @@
   <si>
     <t>Completed On</t>
   </si>
+  <si>
+    <t>Git Uploded</t>
+  </si>
 </sst>
 </file>
 
@@ -141,7 +144,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -180,6 +183,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -220,7 +228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -252,6 +260,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -267,6 +276,2340 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp10.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp11.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp13.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp14.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp15.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp16.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp17.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp18.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp19.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp20.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp21.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp22.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp23.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp24.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp25.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp26.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp27.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp28.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp9.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>276225</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>1085850</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1026" name="Check Box 2" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1026"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>Git Uploded</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>276225</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="809625" cy="209550"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1043" name="Check Box 19" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1043"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>Git Uploded</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>276225</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="809625" cy="209550"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1044" name="Check Box 20" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1044"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>Git Uploded</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>276225</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="809625" cy="209550"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1045" name="Check Box 21" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1045"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>Git Uploded</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>276225</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="809625" cy="209550"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1046" name="Check Box 22" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1046"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>Git Uploded</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>276225</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="809625" cy="209550"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1047" name="Check Box 23" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1047"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>Git Uploded</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>276225</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="809625" cy="209550"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1048" name="Check Box 24" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1048"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>Git Uploded</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>276225</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="809625" cy="209550"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1049" name="Check Box 25" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1049"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>Git Uploded</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>276225</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="809625" cy="209550"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1050" name="Check Box 26" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1050"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>Git Uploded</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>276225</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="809625" cy="209550"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1051" name="Check Box 27" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1051"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>Git Uploded</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>276225</xdr:colOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="809625" cy="209550"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1052" name="Check Box 28" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1052"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>Git Uploded</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>276225</xdr:colOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="809625" cy="209550"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1053" name="Check Box 29" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1053"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>Git Uploded</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>276225</xdr:colOff>
+          <xdr:row>14</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="809625" cy="209550"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1054" name="Check Box 30" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1054"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>Git Uploded</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>276225</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="809625" cy="209550"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1055" name="Check Box 31" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1055"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>Git Uploded</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>276225</xdr:colOff>
+          <xdr:row>16</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="809625" cy="209550"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1056" name="Check Box 32" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1056"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>Git Uploded</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>276225</xdr:colOff>
+          <xdr:row>17</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="809625" cy="209550"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1057" name="Check Box 33" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1057"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>Git Uploded</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>276225</xdr:colOff>
+          <xdr:row>18</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="809625" cy="209550"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1058" name="Check Box 34" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1058"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>Git Uploded</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>276225</xdr:colOff>
+          <xdr:row>19</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="809625" cy="209550"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1059" name="Check Box 35" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1059"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>Git Uploded</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>276225</xdr:colOff>
+          <xdr:row>20</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="809625" cy="209550"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1060" name="Check Box 36" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1060"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>Git Uploded</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>276225</xdr:colOff>
+          <xdr:row>21</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="809625" cy="209550"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1061" name="Check Box 37" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1061"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>Git Uploded</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>276225</xdr:colOff>
+          <xdr:row>22</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="809625" cy="209550"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1062" name="Check Box 38" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1062"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>Git Uploded</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>276225</xdr:colOff>
+          <xdr:row>23</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="809625" cy="209550"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1063" name="Check Box 39" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1063"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>Git Uploded</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>276225</xdr:colOff>
+          <xdr:row>24</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="809625" cy="209550"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1064" name="Check Box 40" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1064"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>Git Uploded</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>276225</xdr:colOff>
+          <xdr:row>25</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="809625" cy="209550"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1065" name="Check Box 41" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1065"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>Git Uploded</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>276225</xdr:colOff>
+          <xdr:row>26</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="809625" cy="209550"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1066" name="Check Box 42" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1066"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>Git Uploded</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>276225</xdr:colOff>
+          <xdr:row>27</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="809625" cy="209550"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1067" name="Check Box 43" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1067"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>Git Uploded</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>276225</xdr:colOff>
+          <xdr:row>28</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="809625" cy="209550"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1068" name="Check Box 44" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1068"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>Git Uploded</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>276225</xdr:colOff>
+          <xdr:row>29</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="809625" cy="209550"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1069" name="Check Box 45" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1069"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>Git Uploded</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -531,11 +2874,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,10 +2886,11 @@
     <col min="1" max="1" width="10.28515625" customWidth="1"/>
     <col min="2" max="2" width="57.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -555,8 +2899,9 @@
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -566,11 +2911,14 @@
       <c r="C2" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -580,11 +2928,12 @@
       <c r="C3" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="15"/>
+      <c r="E3" s="10">
         <v>43927</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -594,11 +2943,12 @@
       <c r="C4" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="15"/>
+      <c r="E4" s="10">
         <v>43929</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>3</v>
       </c>
@@ -608,11 +2958,12 @@
       <c r="C5" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="15"/>
+      <c r="E5" s="10">
         <v>43929</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>4</v>
       </c>
@@ -622,11 +2973,12 @@
       <c r="C6" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="15"/>
+      <c r="E6" s="10">
         <v>43934</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -636,8 +2988,12 @@
       <c r="C7" s="9" t="s">
         <v>32</v>
       </c>
+      <c r="D7" s="15"/>
+      <c r="E7" s="10">
+        <v>43935</v>
+      </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>6</v>
       </c>
@@ -647,8 +3003,9 @@
       <c r="C8" s="9" t="s">
         <v>32</v>
       </c>
+      <c r="D8" s="15"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>7</v>
       </c>
@@ -658,8 +3015,9 @@
       <c r="C9" s="9" t="s">
         <v>32</v>
       </c>
+      <c r="D9" s="15"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>8</v>
       </c>
@@ -669,8 +3027,9 @@
       <c r="C10" s="8" t="s">
         <v>33</v>
       </c>
+      <c r="D10" s="15"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>9</v>
       </c>
@@ -680,8 +3039,9 @@
       <c r="C11" s="8" t="s">
         <v>33</v>
       </c>
+      <c r="D11" s="15"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>10</v>
       </c>
@@ -691,8 +3051,9 @@
       <c r="C12" s="9" t="s">
         <v>32</v>
       </c>
+      <c r="D12" s="15"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>11</v>
       </c>
@@ -702,8 +3063,9 @@
       <c r="C13" s="9" t="s">
         <v>32</v>
       </c>
+      <c r="D13" s="15"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>12</v>
       </c>
@@ -713,8 +3075,9 @@
       <c r="C14" s="8" t="s">
         <v>33</v>
       </c>
+      <c r="D14" s="15"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>13</v>
       </c>
@@ -724,8 +3087,9 @@
       <c r="C15" s="9" t="s">
         <v>32</v>
       </c>
+      <c r="D15" s="15"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>14</v>
       </c>
@@ -735,8 +3099,9 @@
       <c r="C16" s="9" t="s">
         <v>32</v>
       </c>
+      <c r="D16" s="15"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>15</v>
       </c>
@@ -746,8 +3111,9 @@
       <c r="C17" s="9" t="s">
         <v>32</v>
       </c>
+      <c r="D17" s="15"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>16</v>
       </c>
@@ -757,8 +3123,9 @@
       <c r="C18" s="9" t="s">
         <v>32</v>
       </c>
+      <c r="D18" s="15"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>17</v>
       </c>
@@ -768,8 +3135,9 @@
       <c r="C19" s="8" t="s">
         <v>33</v>
       </c>
+      <c r="D19" s="15"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>18</v>
       </c>
@@ -779,8 +3147,9 @@
       <c r="C20" s="8" t="s">
         <v>33</v>
       </c>
+      <c r="D20" s="15"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>19</v>
       </c>
@@ -790,8 +3159,9 @@
       <c r="C21" s="9" t="s">
         <v>32</v>
       </c>
+      <c r="D21" s="15"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>20</v>
       </c>
@@ -801,8 +3171,9 @@
       <c r="C22" s="9" t="s">
         <v>32</v>
       </c>
+      <c r="D22" s="15"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>21</v>
       </c>
@@ -812,8 +3183,9 @@
       <c r="C23" s="9" t="s">
         <v>32</v>
       </c>
+      <c r="D23" s="15"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>22</v>
       </c>
@@ -823,8 +3195,9 @@
       <c r="C24" s="9" t="s">
         <v>32</v>
       </c>
+      <c r="D24" s="15"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>23</v>
       </c>
@@ -834,8 +3207,9 @@
       <c r="C25" s="9" t="s">
         <v>32</v>
       </c>
+      <c r="D25" s="15"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>24</v>
       </c>
@@ -845,8 +3219,9 @@
       <c r="C26" s="9" t="s">
         <v>32</v>
       </c>
+      <c r="D26" s="15"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>25</v>
       </c>
@@ -856,8 +3231,9 @@
       <c r="C27" s="9" t="s">
         <v>32</v>
       </c>
+      <c r="D27" s="15"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>26</v>
       </c>
@@ -867,8 +3243,9 @@
       <c r="C28" s="8" t="s">
         <v>33</v>
       </c>
+      <c r="D28" s="15"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>27</v>
       </c>
@@ -878,8 +3255,9 @@
       <c r="C29" s="9" t="s">
         <v>32</v>
       </c>
+      <c r="D29" s="15"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>28</v>
       </c>
@@ -889,14 +3267,639 @@
       <c r="C30" s="8" t="s">
         <v>33</v>
       </c>
+      <c r="D30" s="15"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:D30">
+  <autoFilter ref="A2:E30">
     <sortState ref="A3:D30">
       <sortCondition ref="A2:A30"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1026" r:id="rId4" name="Check Box 2">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>276225</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>1085850</xdr:colOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1043" r:id="rId5" name="Check Box 19">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>276225</xdr:colOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>1085850</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1044" r:id="rId6" name="Check Box 20">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>276225</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>1085850</xdr:colOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1045" r:id="rId7" name="Check Box 21">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>276225</xdr:colOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>1085850</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1046" r:id="rId8" name="Check Box 22">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>276225</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>1085850</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1047" r:id="rId9" name="Check Box 23">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>276225</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>1085850</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1048" r:id="rId10" name="Check Box 24">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>276225</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>1085850</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1049" r:id="rId11" name="Check Box 25">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>276225</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>1085850</xdr:colOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1050" r:id="rId12" name="Check Box 26">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>276225</xdr:colOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>1085850</xdr:colOff>
+                    <xdr:row>11</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1051" r:id="rId13" name="Check Box 27">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>276225</xdr:colOff>
+                    <xdr:row>11</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>1085850</xdr:colOff>
+                    <xdr:row>12</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1052" r:id="rId14" name="Check Box 28">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>276225</xdr:colOff>
+                    <xdr:row>12</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>1085850</xdr:colOff>
+                    <xdr:row>13</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1053" r:id="rId15" name="Check Box 29">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>276225</xdr:colOff>
+                    <xdr:row>13</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>1085850</xdr:colOff>
+                    <xdr:row>14</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1054" r:id="rId16" name="Check Box 30">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>276225</xdr:colOff>
+                    <xdr:row>14</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>1085850</xdr:colOff>
+                    <xdr:row>15</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1055" r:id="rId17" name="Check Box 31">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>276225</xdr:colOff>
+                    <xdr:row>15</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>1085850</xdr:colOff>
+                    <xdr:row>16</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1056" r:id="rId18" name="Check Box 32">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>276225</xdr:colOff>
+                    <xdr:row>16</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>1085850</xdr:colOff>
+                    <xdr:row>17</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1057" r:id="rId19" name="Check Box 33">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>276225</xdr:colOff>
+                    <xdr:row>17</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>1085850</xdr:colOff>
+                    <xdr:row>18</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1058" r:id="rId20" name="Check Box 34">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>276225</xdr:colOff>
+                    <xdr:row>18</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>1085850</xdr:colOff>
+                    <xdr:row>19</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1059" r:id="rId21" name="Check Box 35">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>276225</xdr:colOff>
+                    <xdr:row>19</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>1085850</xdr:colOff>
+                    <xdr:row>20</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1060" r:id="rId22" name="Check Box 36">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>276225</xdr:colOff>
+                    <xdr:row>20</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>1085850</xdr:colOff>
+                    <xdr:row>21</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1061" r:id="rId23" name="Check Box 37">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>276225</xdr:colOff>
+                    <xdr:row>21</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>1085850</xdr:colOff>
+                    <xdr:row>22</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1062" r:id="rId24" name="Check Box 38">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>276225</xdr:colOff>
+                    <xdr:row>22</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>1085850</xdr:colOff>
+                    <xdr:row>23</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1063" r:id="rId25" name="Check Box 39">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>276225</xdr:colOff>
+                    <xdr:row>23</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>1085850</xdr:colOff>
+                    <xdr:row>24</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1064" r:id="rId26" name="Check Box 40">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>276225</xdr:colOff>
+                    <xdr:row>24</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>1085850</xdr:colOff>
+                    <xdr:row>25</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1065" r:id="rId27" name="Check Box 41">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>276225</xdr:colOff>
+                    <xdr:row>25</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>1085850</xdr:colOff>
+                    <xdr:row>26</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1066" r:id="rId28" name="Check Box 42">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>276225</xdr:colOff>
+                    <xdr:row>26</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>1085850</xdr:colOff>
+                    <xdr:row>27</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1067" r:id="rId29" name="Check Box 43">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>276225</xdr:colOff>
+                    <xdr:row>27</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>1085850</xdr:colOff>
+                    <xdr:row>28</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1068" r:id="rId30" name="Check Box 44">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>276225</xdr:colOff>
+                    <xdr:row>28</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>1085850</xdr:colOff>
+                    <xdr:row>29</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1069" r:id="rId31" name="Check Box 45">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>276225</xdr:colOff>
+                    <xdr:row>29</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>1085850</xdr:colOff>
+                    <xdr:row>30</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
 </worksheet>
 </file>
</xml_diff>